<commit_message>
Adding the 4 test files
</commit_message>
<xml_diff>
--- a/inst/data/475treatedDataset.xlsx
+++ b/inst/data/475treatedDataset.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fcordero/Documents/RunProject/AIRC2015-DiRenzo/RunsMay2019/475Trt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susie/Documents/Ricerca/Francesca/ConfrontiFunctionalClustering/2022/Dati/475Trt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697F71CD-B97C-CA4D-8D0A-C53B49524432}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{937A5A51-9FFD-954A-8D5E-3C763382B547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="475treated_GrowDataFile" sheetId="1" r:id="rId1"/>
+    <sheet name="475treated_less2000_GrowDataFil" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="30" uniqueCount="16">
   <si>
     <t>time</t>
   </si>
@@ -78,39 +87,530 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <start/>
+      <end/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color rgb="FF7F7F7F"/>
+      </start>
+      <end style="thin">
+        <color rgb="FF7F7F7F"/>
+      </end>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color rgb="FF3F3F3F"/>
+      </start>
+      <end style="thin">
+        <color rgb="FF3F3F3F"/>
+      </end>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="double">
+        <color rgb="FF3F3F3F"/>
+      </start>
+      <end style="double">
+        <color rgb="FF3F3F3F"/>
+      </end>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color rgb="FFB2B2B2"/>
+      </start>
+      <end style="thin">
+        <color rgb="FFB2B2B2"/>
+      </end>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -126,7 +626,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -279,25 +779,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:lumMod val="110%"/>
+                <a:satMod val="105%"/>
+                <a:tint val="67%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="103%"/>
+                <a:tint val="73%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="109%"/>
+                <a:tint val="81%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -305,25 +805,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:satMod val="103%"/>
+                <a:lumMod val="102%"/>
+                <a:tint val="94%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:satMod val="110%"/>
+                <a:lumMod val="100%"/>
+                <a:shade val="100%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:lumMod val="99%"/>
+                <a:satMod val="120%"/>
+                <a:shade val="78%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -336,21 +836,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -364,7 +864,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="63%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -376,32 +876,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
+            <a:tint val="95%"/>
+            <a:satMod val="170%"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="93%"/>
+                <a:satMod val="150%"/>
+                <a:shade val="98%"/>
+                <a:lumMod val="102%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="98%"/>
+                <a:satMod val="130%"/>
+                <a:shade val="90%"/>
+                <a:lumMod val="103%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="63%"/>
+                <a:satMod val="120%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -421,49 +921,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
-    <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="5" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" customWidth="1"/>
-    <col min="7" max="7" width="5" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" customWidth="1"/>
-    <col min="9" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" customWidth="1"/>
-    <col min="11" max="11" width="5" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" customWidth="1"/>
-    <col min="13" max="13" width="5" customWidth="1"/>
-    <col min="14" max="14" width="11.83203125" customWidth="1"/>
-    <col min="15" max="15" width="5" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" customWidth="1"/>
-    <col min="17" max="17" width="5" customWidth="1"/>
-    <col min="18" max="18" width="11.83203125" customWidth="1"/>
-    <col min="19" max="19" width="5" customWidth="1"/>
-    <col min="20" max="20" width="11.83203125" customWidth="1"/>
-    <col min="21" max="21" width="5" customWidth="1"/>
-    <col min="22" max="22" width="11.83203125" customWidth="1"/>
-    <col min="23" max="23" width="5" customWidth="1"/>
-    <col min="24" max="24" width="11.83203125" customWidth="1"/>
-    <col min="25" max="25" width="5" customWidth="1"/>
-    <col min="26" max="26" width="11.83203125" customWidth="1"/>
-    <col min="27" max="27" width="5" customWidth="1"/>
-    <col min="28" max="28" width="11.83203125" customWidth="1"/>
-    <col min="29" max="29" width="5" customWidth="1"/>
-    <col min="30" max="30" width="11.83203125" customWidth="1"/>
-    <col min="31" max="1025" width="11.5"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,7 +1022,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -647,7 +1114,7 @@
         <v>179.45959999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
@@ -739,7 +1206,7 @@
         <v>82.410295500000004</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>17</v>
       </c>
@@ -831,7 +1298,7 @@
         <v>97.369062499999998</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>25</v>
       </c>
@@ -923,7 +1390,7 @@
         <v>177.54565400000001</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>31</v>
       </c>
@@ -1015,7 +1482,7 @@
         <v>442.72805849999997</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>35</v>
       </c>
@@ -1107,7 +1574,7 @@
         <v>667.86260400000003</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>38</v>
       </c>
@@ -1199,7 +1666,7 @@
         <v>1065.5728919999999</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>42</v>
       </c>
@@ -1291,7 +1758,7 @@
         <v>1226.743788</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>45</v>
       </c>
@@ -1383,7 +1850,7 @@
         <v>573.78554099999997</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>48</v>
       </c>
@@ -1475,7 +1942,7 @@
         <v>508.62292000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>52</v>
       </c>
@@ -1567,7 +2034,7 @@
         <v>128.69999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>56</v>
       </c>
@@ -1659,7 +2126,7 @@
         <v>104.938106</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>59</v>
       </c>
@@ -1751,7 +2218,7 @@
         <v>37.678888000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>63</v>
       </c>
@@ -1843,7 +2310,7 @@
         <v>180.09337500000001</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>66</v>
       </c>
@@ -1935,7 +2402,7 @@
         <v>96.715874499999998</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>70</v>
       </c>
@@ -2027,7 +2494,7 @@
         <v>76.444654</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>73</v>
       </c>
@@ -2119,7 +2586,7 @@
         <v>154.5615</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>82</v>
       </c>
@@ -2211,7 +2678,7 @@
         <v>617.64764600000001</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>89</v>
       </c>
@@ -2303,7 +2770,7 @@
         <v>857.02610700000002</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>95</v>
       </c>
@@ -2395,7 +2862,7 @@
         <v>778.36946850000004</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>101</v>
       </c>
@@ -2426,24 +2893,12 @@
       <c r="L22">
         <v>727.02691800000002</v>
       </c>
-      <c r="M22">
-        <v>95</v>
-      </c>
-      <c r="N22">
-        <v>2232.0542479999999</v>
-      </c>
       <c r="O22">
         <v>95</v>
       </c>
       <c r="P22">
         <v>1577.8330000000001</v>
       </c>
-      <c r="Q22">
-        <v>95</v>
-      </c>
-      <c r="R22">
-        <v>2334.9288280000001</v>
-      </c>
       <c r="S22">
         <v>101</v>
       </c>
@@ -2481,31 +2936,19 @@
         <v>1464.12</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="G23">
         <v>101</v>
       </c>
       <c r="H23">
         <v>464.22610650000001</v>
       </c>
-      <c r="I23">
-        <v>108</v>
-      </c>
-      <c r="J23">
-        <v>2714.4174979999998</v>
-      </c>
       <c r="O23">
         <v>101</v>
       </c>
       <c r="P23">
         <v>1890.8242250000001</v>
       </c>
-      <c r="Q23">
-        <v>101</v>
-      </c>
-      <c r="R23">
-        <v>4576.1630720000003</v>
-      </c>
       <c r="S23">
         <v>108</v>
       </c>
@@ -2518,20 +2961,8 @@
       <c r="AB23">
         <v>1049.8607959999999</v>
       </c>
-      <c r="AC23">
-        <v>106</v>
-      </c>
-      <c r="AD23">
-        <v>2268.5888060000002</v>
-      </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="I24">
-        <v>115</v>
-      </c>
-      <c r="J24">
-        <v>3937.0538959999999</v>
-      </c>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="S24">
         <v>115</v>
       </c>
@@ -2544,33 +2975,16 @@
       <c r="AB24">
         <v>1166.152198</v>
       </c>
-      <c r="AC24">
-        <v>112</v>
-      </c>
-      <c r="AD24">
-        <v>2548.5045759999998</v>
-      </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="AA25">
         <v>118</v>
       </c>
       <c r="AB25">
         <v>1385.7029729999999</v>
       </c>
-      <c r="AC25">
-        <v>118</v>
-      </c>
-      <c r="AD25">
-        <v>2877.1959919999999</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>